<commit_message>
Started with datagid formatting for config
</commit_message>
<xml_diff>
--- a/Booyco HMI Utility/Resources/Documents/CommanderParametersFile.xlsx
+++ b/Booyco HMI Utility/Resources/Documents/CommanderParametersFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Neil\Dropbox (Mernok Elektronik)\Software\Booyco HMI Utility\Booyco HMI Utility\Resources\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5116A9C-131A-458D-9EC9-EF454E351A7D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254F9DA3-6C9B-4887-AD8E-644631C04EDD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4442C273-631E-40E6-88D2-7449766A5078}"/>
+    <workbookView xWindow="630" yWindow="2475" windowWidth="24840" windowHeight="11385" xr2:uid="{4442C273-631E-40E6-88D2-7449766A5078}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1676,8 +1676,8 @@
   <dimension ref="A1:N317"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K292" sqref="K292"/>
+      <pane ySplit="1" topLeftCell="A287" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F290" sqref="F290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9095,10 +9095,10 @@
         <v>0</v>
       </c>
       <c r="F289" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G289" s="3">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.25">
@@ -9119,10 +9119,10 @@
         <v>0</v>
       </c>
       <c r="F290" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G290" s="3">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.25">
@@ -9143,10 +9143,10 @@
         <v>3</v>
       </c>
       <c r="F291" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G291" s="3">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Stable Heartbeat for wifi
</commit_message>
<xml_diff>
--- a/Booyco HMI Utility/Resources/Documents/CommanderParametersFile.xlsx
+++ b/Booyco HMI Utility/Resources/Documents/CommanderParametersFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Neil\Dropbox (Mernok Elektronik)\Software\Booyco HMI Utility\Booyco HMI Utility\Resources\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA909C25-E83B-44E0-9204-7DAD6DEF92E1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D01648-B82F-42EE-B595-35C035904350}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="840" windowWidth="24840" windowHeight="11385" xr2:uid="{4442C273-631E-40E6-88D2-7449766A5078}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4442C273-631E-40E6-88D2-7449766A5078}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="422">
   <si>
     <t>Name</t>
   </si>
@@ -1285,6 +1285,18 @@
   </si>
   <si>
     <t>Periferals</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Firmware sub-revision of the device, used to indicate minor updates</t>
+  </si>
+  <si>
+    <t>Firmware revision of the device used to indicate major updates and possible compatibility issues</t>
+  </si>
+  <si>
+    <t>No Info</t>
   </si>
 </sst>
 </file>
@@ -1726,11 +1738,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4E73DD7-587F-4C4F-B32B-7B78C2644041}">
-  <dimension ref="A1:N317"/>
+  <dimension ref="A1:P317"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
+      <selection pane="bottomLeft" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,13 +1752,14 @@
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="89" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1774,11 +1787,8 @@
       <c r="I1" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>378</v>
+      <c r="J1" s="6" t="s">
+        <v>418</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>9</v>
@@ -1786,8 +1796,14 @@
       <c r="N1" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>70</v>
       </c>
@@ -1816,11 +1832,8 @@
       <c r="I2" t="s">
         <v>413</v>
       </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>376</v>
+      <c r="J2" t="s">
+        <v>420</v>
       </c>
       <c r="M2" s="1">
         <v>1</v>
@@ -1828,8 +1841,14 @@
       <c r="N2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="2">
+        <v>0</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>71</v>
       </c>
@@ -1858,11 +1877,8 @@
       <c r="I3" t="s">
         <v>413</v>
       </c>
-      <c r="J3" s="2">
-        <v>1</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>377</v>
+      <c r="J3" t="s">
+        <v>419</v>
       </c>
       <c r="M3" s="1">
         <v>1</v>
@@ -1870,8 +1886,14 @@
       <c r="N3" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="2">
+        <v>1</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1900,11 +1922,8 @@
       <c r="I4" t="s">
         <v>413</v>
       </c>
-      <c r="J4" s="2">
-        <v>2</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>9</v>
+      <c r="J4" t="s">
+        <v>421</v>
       </c>
       <c r="M4" s="1">
         <v>1</v>
@@ -1912,8 +1931,14 @@
       <c r="N4" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" s="2">
+        <v>2</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1942,11 +1967,8 @@
       <c r="I5" t="s">
         <v>413</v>
       </c>
-      <c r="J5" s="4">
-        <v>4</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>379</v>
+      <c r="J5" t="s">
+        <v>421</v>
       </c>
       <c r="M5" s="1">
         <v>1</v>
@@ -1954,8 +1976,14 @@
       <c r="N5" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" s="4">
+        <v>4</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1984,6 +2012,9 @@
       <c r="I6" t="s">
         <v>413</v>
       </c>
+      <c r="J6" t="s">
+        <v>421</v>
+      </c>
       <c r="M6" s="1">
         <v>2</v>
       </c>
@@ -1991,7 +2022,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>63</v>
       </c>
@@ -2020,6 +2051,9 @@
       <c r="I7" t="s">
         <v>413</v>
       </c>
+      <c r="J7" t="s">
+        <v>421</v>
+      </c>
       <c r="M7" s="1">
         <v>2</v>
       </c>
@@ -2027,7 +2061,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>72</v>
       </c>
@@ -2056,6 +2090,9 @@
       <c r="I8" t="s">
         <v>413</v>
       </c>
+      <c r="J8" t="s">
+        <v>421</v>
+      </c>
       <c r="M8" s="1">
         <v>3</v>
       </c>
@@ -2063,7 +2100,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>73</v>
       </c>
@@ -2092,6 +2129,9 @@
       <c r="I9" t="s">
         <v>413</v>
       </c>
+      <c r="J9" t="s">
+        <v>421</v>
+      </c>
       <c r="M9" s="1">
         <v>4</v>
       </c>
@@ -2099,7 +2139,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>74</v>
       </c>
@@ -2128,6 +2168,9 @@
       <c r="I10" t="s">
         <v>413</v>
       </c>
+      <c r="J10" t="s">
+        <v>421</v>
+      </c>
       <c r="M10" s="1">
         <v>4</v>
       </c>
@@ -2135,7 +2178,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>75</v>
       </c>
@@ -2164,6 +2207,9 @@
       <c r="I11" t="s">
         <v>413</v>
       </c>
+      <c r="J11" t="s">
+        <v>421</v>
+      </c>
       <c r="M11" s="1">
         <v>4</v>
       </c>
@@ -2171,7 +2217,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>76</v>
       </c>
@@ -2200,6 +2246,9 @@
       <c r="I12" t="s">
         <v>413</v>
       </c>
+      <c r="J12" t="s">
+        <v>421</v>
+      </c>
       <c r="M12" s="1">
         <v>4</v>
       </c>
@@ -2207,7 +2256,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>77</v>
       </c>
@@ -2236,6 +2285,9 @@
       <c r="I13" t="s">
         <v>413</v>
       </c>
+      <c r="J13" t="s">
+        <v>421</v>
+      </c>
       <c r="M13" s="1">
         <v>4</v>
       </c>
@@ -2243,7 +2295,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>78</v>
       </c>
@@ -2272,6 +2324,9 @@
       <c r="I14" t="s">
         <v>413</v>
       </c>
+      <c r="J14" t="s">
+        <v>421</v>
+      </c>
       <c r="M14" s="1">
         <v>5</v>
       </c>
@@ -2279,7 +2334,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>79</v>
       </c>
@@ -2308,6 +2363,9 @@
       <c r="I15" t="s">
         <v>413</v>
       </c>
+      <c r="J15" t="s">
+        <v>421</v>
+      </c>
       <c r="M15" s="1">
         <v>5</v>
       </c>
@@ -2315,7 +2373,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>80</v>
       </c>
@@ -2344,6 +2402,9 @@
       <c r="I16" t="s">
         <v>413</v>
       </c>
+      <c r="J16" t="s">
+        <v>421</v>
+      </c>
       <c r="M16" s="1">
         <v>5</v>
       </c>
@@ -2380,6 +2441,9 @@
       <c r="I17" t="s">
         <v>413</v>
       </c>
+      <c r="J17" t="s">
+        <v>421</v>
+      </c>
       <c r="M17" s="1">
         <v>5</v>
       </c>
@@ -2416,6 +2480,9 @@
       <c r="I18" t="s">
         <v>413</v>
       </c>
+      <c r="J18" t="s">
+        <v>421</v>
+      </c>
       <c r="M18" s="1">
         <v>5</v>
       </c>
@@ -2452,6 +2519,9 @@
       <c r="I19" t="s">
         <v>413</v>
       </c>
+      <c r="J19" t="s">
+        <v>421</v>
+      </c>
       <c r="M19" s="1">
         <v>6</v>
       </c>
@@ -2488,6 +2558,9 @@
       <c r="I20" t="s">
         <v>413</v>
       </c>
+      <c r="J20" t="s">
+        <v>421</v>
+      </c>
       <c r="M20" s="1">
         <v>6</v>
       </c>
@@ -2524,6 +2597,9 @@
       <c r="I21" t="s">
         <v>413</v>
       </c>
+      <c r="J21" t="s">
+        <v>421</v>
+      </c>
       <c r="M21" s="1">
         <v>6</v>
       </c>
@@ -2560,6 +2636,9 @@
       <c r="I22" t="s">
         <v>413</v>
       </c>
+      <c r="J22" t="s">
+        <v>421</v>
+      </c>
       <c r="M22" s="1">
         <v>6</v>
       </c>
@@ -2596,6 +2675,9 @@
       <c r="I23" t="s">
         <v>413</v>
       </c>
+      <c r="J23" t="s">
+        <v>421</v>
+      </c>
       <c r="M23" s="1">
         <v>6</v>
       </c>
@@ -2632,6 +2714,9 @@
       <c r="I24" t="s">
         <v>413</v>
       </c>
+      <c r="J24" t="s">
+        <v>421</v>
+      </c>
       <c r="M24" s="1">
         <v>6</v>
       </c>
@@ -2668,6 +2753,9 @@
       <c r="I25" t="s">
         <v>413</v>
       </c>
+      <c r="J25" t="s">
+        <v>421</v>
+      </c>
       <c r="M25" s="1">
         <v>6</v>
       </c>
@@ -2704,6 +2792,9 @@
       <c r="I26" t="s">
         <v>413</v>
       </c>
+      <c r="J26" t="s">
+        <v>421</v>
+      </c>
       <c r="M26" s="1">
         <v>6</v>
       </c>
@@ -2740,6 +2831,9 @@
       <c r="I27" t="s">
         <v>413</v>
       </c>
+      <c r="J27" t="s">
+        <v>421</v>
+      </c>
       <c r="M27" s="1">
         <v>6</v>
       </c>
@@ -2776,6 +2870,9 @@
       <c r="I28" t="s">
         <v>414</v>
       </c>
+      <c r="J28" t="s">
+        <v>421</v>
+      </c>
       <c r="M28" s="1">
         <v>6</v>
       </c>
@@ -2812,6 +2909,9 @@
       <c r="I29" t="s">
         <v>414</v>
       </c>
+      <c r="J29" t="s">
+        <v>421</v>
+      </c>
       <c r="M29" s="1">
         <v>7</v>
       </c>
@@ -2848,6 +2948,9 @@
       <c r="I30" t="s">
         <v>414</v>
       </c>
+      <c r="J30" t="s">
+        <v>421</v>
+      </c>
       <c r="M30" s="1">
         <v>7</v>
       </c>
@@ -2884,6 +2987,9 @@
       <c r="I31" t="s">
         <v>414</v>
       </c>
+      <c r="J31" t="s">
+        <v>421</v>
+      </c>
       <c r="M31" s="1">
         <v>7</v>
       </c>
@@ -2920,6 +3026,9 @@
       <c r="I32" t="s">
         <v>413</v>
       </c>
+      <c r="J32" t="s">
+        <v>421</v>
+      </c>
       <c r="M32" s="1">
         <v>7</v>
       </c>
@@ -2956,6 +3065,9 @@
       <c r="I33" t="s">
         <v>413</v>
       </c>
+      <c r="J33" t="s">
+        <v>421</v>
+      </c>
       <c r="M33" s="1">
         <v>7</v>
       </c>
@@ -2992,6 +3104,9 @@
       <c r="I34" t="s">
         <v>413</v>
       </c>
+      <c r="J34" t="s">
+        <v>421</v>
+      </c>
       <c r="M34" s="1">
         <v>7</v>
       </c>
@@ -3028,6 +3143,9 @@
       <c r="I35" t="s">
         <v>413</v>
       </c>
+      <c r="J35" t="s">
+        <v>421</v>
+      </c>
       <c r="M35" s="1">
         <v>7</v>
       </c>
@@ -3064,6 +3182,9 @@
       <c r="I36" t="s">
         <v>413</v>
       </c>
+      <c r="J36" t="s">
+        <v>421</v>
+      </c>
       <c r="M36" s="1">
         <v>7</v>
       </c>
@@ -3100,6 +3221,9 @@
       <c r="I37" t="s">
         <v>415</v>
       </c>
+      <c r="J37" t="s">
+        <v>421</v>
+      </c>
       <c r="M37" s="1">
         <v>7</v>
       </c>
@@ -3136,6 +3260,9 @@
       <c r="I38" t="s">
         <v>415</v>
       </c>
+      <c r="J38" t="s">
+        <v>421</v>
+      </c>
       <c r="M38" s="1">
         <v>7</v>
       </c>
@@ -3172,6 +3299,9 @@
       <c r="I39" t="s">
         <v>415</v>
       </c>
+      <c r="J39" t="s">
+        <v>421</v>
+      </c>
       <c r="M39" s="1">
         <v>7</v>
       </c>
@@ -3208,6 +3338,9 @@
       <c r="I40" t="s">
         <v>415</v>
       </c>
+      <c r="J40" t="s">
+        <v>421</v>
+      </c>
       <c r="M40" s="1">
         <v>7</v>
       </c>
@@ -3244,6 +3377,9 @@
       <c r="I41" t="s">
         <v>416</v>
       </c>
+      <c r="J41" t="s">
+        <v>421</v>
+      </c>
       <c r="M41" s="1">
         <v>8</v>
       </c>
@@ -3280,6 +3416,9 @@
       <c r="I42" t="s">
         <v>416</v>
       </c>
+      <c r="J42" t="s">
+        <v>421</v>
+      </c>
       <c r="M42" s="1">
         <v>8</v>
       </c>
@@ -3316,6 +3455,9 @@
       <c r="I43" t="s">
         <v>416</v>
       </c>
+      <c r="J43" t="s">
+        <v>421</v>
+      </c>
       <c r="M43" s="1">
         <v>8</v>
       </c>
@@ -3352,6 +3494,9 @@
       <c r="I44" t="s">
         <v>416</v>
       </c>
+      <c r="J44" t="s">
+        <v>421</v>
+      </c>
       <c r="M44" s="1">
         <v>8</v>
       </c>
@@ -3388,6 +3533,9 @@
       <c r="I45" t="s">
         <v>416</v>
       </c>
+      <c r="J45" t="s">
+        <v>421</v>
+      </c>
       <c r="M45" s="1">
         <v>8</v>
       </c>
@@ -3424,6 +3572,9 @@
       <c r="I46" s="5" t="s">
         <v>405</v>
       </c>
+      <c r="J46" t="s">
+        <v>421</v>
+      </c>
       <c r="M46" s="1">
         <v>8</v>
       </c>
@@ -3460,6 +3611,9 @@
       <c r="I47" s="5" t="s">
         <v>405</v>
       </c>
+      <c r="J47" t="s">
+        <v>421</v>
+      </c>
       <c r="M47" s="1">
         <v>8</v>
       </c>
@@ -3496,6 +3650,9 @@
       <c r="I48" s="5" t="s">
         <v>405</v>
       </c>
+      <c r="J48" t="s">
+        <v>421</v>
+      </c>
       <c r="M48" s="1">
         <v>8</v>
       </c>
@@ -3532,6 +3689,9 @@
       <c r="I49" s="5" t="s">
         <v>405</v>
       </c>
+      <c r="J49" t="s">
+        <v>421</v>
+      </c>
       <c r="M49" s="1">
         <v>8</v>
       </c>
@@ -3568,6 +3728,9 @@
       <c r="I50" s="5" t="s">
         <v>405</v>
       </c>
+      <c r="J50" t="s">
+        <v>421</v>
+      </c>
       <c r="M50" s="1">
         <v>8</v>
       </c>
@@ -3604,6 +3767,9 @@
       <c r="I51" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J51" t="s">
+        <v>421</v>
+      </c>
       <c r="M51" s="1">
         <v>8</v>
       </c>
@@ -3640,6 +3806,9 @@
       <c r="I52" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J52" t="s">
+        <v>421</v>
+      </c>
       <c r="M52" s="1">
         <v>8</v>
       </c>
@@ -3676,6 +3845,9 @@
       <c r="I53" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J53" t="s">
+        <v>421</v>
+      </c>
       <c r="M53" s="1">
         <v>8</v>
       </c>
@@ -3712,6 +3884,9 @@
       <c r="I54" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J54" t="s">
+        <v>421</v>
+      </c>
       <c r="M54" s="1">
         <v>8</v>
       </c>
@@ -3748,6 +3923,9 @@
       <c r="I55" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J55" t="s">
+        <v>421</v>
+      </c>
       <c r="M55" s="1">
         <v>8</v>
       </c>
@@ -3784,6 +3962,9 @@
       <c r="I56" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J56" t="s">
+        <v>421</v>
+      </c>
       <c r="M56" s="1">
         <v>8</v>
       </c>
@@ -3820,6 +4001,9 @@
       <c r="I57" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J57" t="s">
+        <v>421</v>
+      </c>
       <c r="M57" s="1">
         <v>9</v>
       </c>
@@ -3856,6 +4040,9 @@
       <c r="I58" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J58" t="s">
+        <v>421</v>
+      </c>
       <c r="M58" s="1">
         <v>9</v>
       </c>
@@ -3892,6 +4079,9 @@
       <c r="I59" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J59" t="s">
+        <v>421</v>
+      </c>
       <c r="M59" s="1">
         <v>10</v>
       </c>
@@ -3928,6 +4118,9 @@
       <c r="I60" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J60" t="s">
+        <v>421</v>
+      </c>
       <c r="M60" s="1">
         <v>10</v>
       </c>
@@ -3964,6 +4157,9 @@
       <c r="I61" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J61" t="s">
+        <v>421</v>
+      </c>
       <c r="M61" s="1">
         <v>10</v>
       </c>
@@ -4000,6 +4196,9 @@
       <c r="I62" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J62" t="s">
+        <v>421</v>
+      </c>
       <c r="M62" s="1">
         <v>10</v>
       </c>
@@ -4036,6 +4235,9 @@
       <c r="I63" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J63" t="s">
+        <v>421</v>
+      </c>
       <c r="M63" s="1">
         <v>11</v>
       </c>
@@ -4072,6 +4274,9 @@
       <c r="I64" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J64" t="s">
+        <v>421</v>
+      </c>
       <c r="M64" s="1">
         <v>11</v>
       </c>
@@ -4108,6 +4313,9 @@
       <c r="I65" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J65" t="s">
+        <v>421</v>
+      </c>
       <c r="M65" s="1">
         <v>11</v>
       </c>
@@ -4144,6 +4352,9 @@
       <c r="I66" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J66" t="s">
+        <v>421</v>
+      </c>
       <c r="M66" s="1">
         <v>11</v>
       </c>
@@ -4180,6 +4391,9 @@
       <c r="I67" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J67" t="s">
+        <v>421</v>
+      </c>
       <c r="M67" s="1">
         <v>11</v>
       </c>
@@ -4216,6 +4430,9 @@
       <c r="I68" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J68" t="s">
+        <v>421</v>
+      </c>
       <c r="M68" s="1">
         <v>11</v>
       </c>
@@ -4252,6 +4469,9 @@
       <c r="I69" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J69" t="s">
+        <v>421</v>
+      </c>
       <c r="M69" s="1">
         <v>11</v>
       </c>
@@ -4288,6 +4508,9 @@
       <c r="I70" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J70" t="s">
+        <v>421</v>
+      </c>
       <c r="M70" s="1">
         <v>11</v>
       </c>
@@ -4324,6 +4547,9 @@
       <c r="I71" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J71" t="s">
+        <v>421</v>
+      </c>
       <c r="M71" s="1">
         <v>11</v>
       </c>
@@ -4360,6 +4586,9 @@
       <c r="I72" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J72" t="s">
+        <v>421</v>
+      </c>
       <c r="M72" s="1">
         <v>11</v>
       </c>
@@ -4396,6 +4625,9 @@
       <c r="I73" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J73" t="s">
+        <v>421</v>
+      </c>
       <c r="M73" s="1">
         <v>11</v>
       </c>
@@ -4432,6 +4664,9 @@
       <c r="I74" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J74" t="s">
+        <v>421</v>
+      </c>
       <c r="M74" s="1">
         <v>11</v>
       </c>
@@ -4468,6 +4703,9 @@
       <c r="I75" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J75" t="s">
+        <v>421</v>
+      </c>
       <c r="M75" s="1">
         <v>11</v>
       </c>
@@ -4504,6 +4742,9 @@
       <c r="I76" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J76" t="s">
+        <v>421</v>
+      </c>
       <c r="M76" s="1">
         <v>11</v>
       </c>
@@ -4540,6 +4781,9 @@
       <c r="I77" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J77" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
@@ -4570,6 +4814,9 @@
       <c r="I78" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J78" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
@@ -4600,6 +4847,9 @@
       <c r="I79" s="5" t="s">
         <v>406</v>
       </c>
+      <c r="J79" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
@@ -4630,8 +4880,11 @@
       <c r="I80" s="5" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J80" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>142</v>
       </c>
@@ -4660,8 +4913,11 @@
       <c r="I81" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J81" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>143</v>
       </c>
@@ -4690,8 +4946,11 @@
       <c r="I82" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J82" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>144</v>
       </c>
@@ -4720,8 +4979,11 @@
       <c r="I83" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J83" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>145</v>
       </c>
@@ -4750,8 +5012,11 @@
       <c r="I84" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J84" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>146</v>
       </c>
@@ -4780,8 +5045,11 @@
       <c r="I85" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J85" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>147</v>
       </c>
@@ -4810,8 +5078,11 @@
       <c r="I86" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J86" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>148</v>
       </c>
@@ -4840,8 +5111,11 @@
       <c r="I87" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J87" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>149</v>
       </c>
@@ -4870,8 +5144,11 @@
       <c r="I88" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J88" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>150</v>
       </c>
@@ -4900,8 +5177,11 @@
       <c r="I89" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J89" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>151</v>
       </c>
@@ -4930,8 +5210,11 @@
       <c r="I90" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J90" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>152</v>
       </c>
@@ -4960,8 +5243,11 @@
       <c r="I91" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J91" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>153</v>
       </c>
@@ -4990,8 +5276,11 @@
       <c r="I92" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J92" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>154</v>
       </c>
@@ -5020,8 +5309,11 @@
       <c r="I93" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J93" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>155</v>
       </c>
@@ -5050,8 +5342,11 @@
       <c r="I94" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J94" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>156</v>
       </c>
@@ -5080,8 +5375,11 @@
       <c r="I95" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J95" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>157</v>
       </c>
@@ -5110,8 +5408,11 @@
       <c r="I96" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J96" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>158</v>
       </c>
@@ -5140,8 +5441,11 @@
       <c r="I97" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J97" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>159</v>
       </c>
@@ -5170,8 +5474,11 @@
       <c r="I98" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J98" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>160</v>
       </c>
@@ -5200,8 +5507,11 @@
       <c r="I99" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J99" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>161</v>
       </c>
@@ -5230,8 +5540,11 @@
       <c r="I100" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J100" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>162</v>
       </c>
@@ -5260,8 +5573,11 @@
       <c r="I101" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J101" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>163</v>
       </c>
@@ -5290,8 +5606,11 @@
       <c r="I102" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J102" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>164</v>
       </c>
@@ -5320,8 +5639,11 @@
       <c r="I103" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J103" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>165</v>
       </c>
@@ -5350,8 +5672,11 @@
       <c r="I104" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J104" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>166</v>
       </c>
@@ -5380,8 +5705,11 @@
       <c r="I105" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J105" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>167</v>
       </c>
@@ -5410,8 +5738,11 @@
       <c r="I106" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J106" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>168</v>
       </c>
@@ -5440,8 +5771,11 @@
       <c r="I107" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J107" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>169</v>
       </c>
@@ -5470,8 +5804,11 @@
       <c r="I108" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J108" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>170</v>
       </c>
@@ -5500,8 +5837,11 @@
       <c r="I109" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J109" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>171</v>
       </c>
@@ -5530,8 +5870,11 @@
       <c r="I110" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J110" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>172</v>
       </c>
@@ -5560,8 +5903,11 @@
       <c r="I111" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J111" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>173</v>
       </c>
@@ -5590,8 +5936,11 @@
       <c r="I112" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J112" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>174</v>
       </c>
@@ -5620,8 +5969,11 @@
       <c r="I113" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J113" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>175</v>
       </c>
@@ -5650,8 +6002,11 @@
       <c r="I114" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J114" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>176</v>
       </c>
@@ -5680,8 +6035,11 @@
       <c r="I115" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J115" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>177</v>
       </c>
@@ -5710,8 +6068,11 @@
       <c r="I116" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J116" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>178</v>
       </c>
@@ -5740,8 +6101,11 @@
       <c r="I117" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J117" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>179</v>
       </c>
@@ -5770,8 +6134,11 @@
       <c r="I118" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J118" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>180</v>
       </c>
@@ -5800,8 +6167,11 @@
       <c r="I119" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J119" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>181</v>
       </c>
@@ -5830,8 +6200,11 @@
       <c r="I120" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J120" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>182</v>
       </c>
@@ -5860,8 +6233,11 @@
       <c r="I121" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J121" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>183</v>
       </c>
@@ -5890,8 +6266,11 @@
       <c r="I122" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J122" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>184</v>
       </c>
@@ -5920,8 +6299,11 @@
       <c r="I123" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J123" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>185</v>
       </c>
@@ -5950,8 +6332,11 @@
       <c r="I124" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J124" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>186</v>
       </c>
@@ -5980,8 +6365,11 @@
       <c r="I125" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J125" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>187</v>
       </c>
@@ -6010,8 +6398,11 @@
       <c r="I126" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J126" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>188</v>
       </c>
@@ -6040,8 +6431,11 @@
       <c r="I127" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J127" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>189</v>
       </c>
@@ -6070,8 +6464,11 @@
       <c r="I128" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J128" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>190</v>
       </c>
@@ -6100,8 +6497,11 @@
       <c r="I129" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J129" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>191</v>
       </c>
@@ -6130,8 +6530,11 @@
       <c r="I130" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J130" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>192</v>
       </c>
@@ -6160,8 +6563,11 @@
       <c r="I131" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J131" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>193</v>
       </c>
@@ -6190,8 +6596,11 @@
       <c r="I132" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J132" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>194</v>
       </c>
@@ -6220,8 +6629,11 @@
       <c r="I133" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J133" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>195</v>
       </c>
@@ -6250,8 +6662,11 @@
       <c r="I134" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J134" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>196</v>
       </c>
@@ -6280,8 +6695,11 @@
       <c r="I135" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J135" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>197</v>
       </c>
@@ -6310,8 +6728,11 @@
       <c r="I136" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J136" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>198</v>
       </c>
@@ -6340,8 +6761,11 @@
       <c r="I137" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J137" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>199</v>
       </c>
@@ -6370,8 +6794,11 @@
       <c r="I138" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J138" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>200</v>
       </c>
@@ -6400,8 +6827,11 @@
       <c r="I139" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J139" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>201</v>
       </c>
@@ -6430,8 +6860,11 @@
       <c r="I140" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J140" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>202</v>
       </c>
@@ -6460,8 +6893,11 @@
       <c r="I141" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J141" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>203</v>
       </c>
@@ -6490,8 +6926,11 @@
       <c r="I142" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J142" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>204</v>
       </c>
@@ -6520,8 +6959,11 @@
       <c r="I143" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J143" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>205</v>
       </c>
@@ -6550,8 +6992,11 @@
       <c r="I144" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J144" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>206</v>
       </c>
@@ -6580,8 +7025,11 @@
       <c r="I145" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J145" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>207</v>
       </c>
@@ -6610,8 +7058,11 @@
       <c r="I146" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J146" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>208</v>
       </c>
@@ -6640,8 +7091,11 @@
       <c r="I147" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J147" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>209</v>
       </c>
@@ -6670,8 +7124,11 @@
       <c r="I148" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J148" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>210</v>
       </c>
@@ -6700,8 +7157,11 @@
       <c r="I149" s="5" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J149" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>211</v>
       </c>
@@ -6730,8 +7190,11 @@
       <c r="I150" s="5" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J150" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>212</v>
       </c>
@@ -6760,8 +7223,11 @@
       <c r="I151" s="5" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J151" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>213</v>
       </c>
@@ -6790,8 +7256,11 @@
       <c r="I152" s="5" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J152" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>214</v>
       </c>
@@ -6820,8 +7289,11 @@
       <c r="I153" s="5" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J153" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>215</v>
       </c>
@@ -6850,8 +7322,11 @@
       <c r="I154" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J154" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>216</v>
       </c>
@@ -6880,8 +7355,11 @@
       <c r="I155" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J155" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>217</v>
       </c>
@@ -6910,8 +7388,11 @@
       <c r="I156" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J156" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>218</v>
       </c>
@@ -6940,8 +7421,11 @@
       <c r="I157" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J157" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>219</v>
       </c>
@@ -6970,8 +7454,11 @@
       <c r="I158" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J158" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>220</v>
       </c>
@@ -7000,8 +7487,11 @@
       <c r="I159" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J159" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>221</v>
       </c>
@@ -7030,8 +7520,11 @@
       <c r="I160" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J160" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>222</v>
       </c>
@@ -7060,8 +7553,11 @@
       <c r="I161" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J161" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>223</v>
       </c>
@@ -7090,8 +7586,11 @@
       <c r="I162" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J162" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>224</v>
       </c>
@@ -7120,8 +7619,11 @@
       <c r="I163" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J163" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>225</v>
       </c>
@@ -7150,8 +7652,11 @@
       <c r="I164" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J164" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>226</v>
       </c>
@@ -7180,8 +7685,11 @@
       <c r="I165" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J165" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>227</v>
       </c>
@@ -7210,8 +7718,11 @@
       <c r="I166" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J166" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>228</v>
       </c>
@@ -7240,8 +7751,11 @@
       <c r="I167" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J167" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>229</v>
       </c>
@@ -7270,8 +7784,11 @@
       <c r="I168" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J168" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>230</v>
       </c>
@@ -7300,8 +7817,11 @@
       <c r="I169" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J169" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
         <v>231</v>
       </c>
@@ -7330,8 +7850,11 @@
       <c r="I170" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J170" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>232</v>
       </c>
@@ -7360,8 +7883,11 @@
       <c r="I171" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J171" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
         <v>233</v>
       </c>
@@ -7390,8 +7916,11 @@
       <c r="I172" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J172" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
         <v>234</v>
       </c>
@@ -7420,8 +7949,11 @@
       <c r="I173" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J173" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
         <v>235</v>
       </c>
@@ -7450,8 +7982,11 @@
       <c r="I174" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J174" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
         <v>236</v>
       </c>
@@ -7480,8 +8015,11 @@
       <c r="I175" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J175" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
         <v>237</v>
       </c>
@@ -7510,8 +8048,11 @@
       <c r="I176" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J176" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
         <v>238</v>
       </c>
@@ -7540,8 +8081,11 @@
       <c r="I177" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J177" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
         <v>239</v>
       </c>
@@ -7570,8 +8114,11 @@
       <c r="I178" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J178" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
         <v>240</v>
       </c>
@@ -7600,8 +8147,11 @@
       <c r="I179" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J179" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
         <v>241</v>
       </c>
@@ -7630,8 +8180,11 @@
       <c r="I180" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J180" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
         <v>242</v>
       </c>
@@ -7660,8 +8213,11 @@
       <c r="I181" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J181" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
         <v>243</v>
       </c>
@@ -7690,8 +8246,11 @@
       <c r="I182" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J182" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
         <v>244</v>
       </c>
@@ -7720,8 +8279,11 @@
       <c r="I183" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J183" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
         <v>245</v>
       </c>
@@ -7750,8 +8312,11 @@
       <c r="I184" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J184" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
         <v>246</v>
       </c>
@@ -7780,8 +8345,11 @@
       <c r="I185" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J185" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
         <v>247</v>
       </c>
@@ -7810,8 +8378,11 @@
       <c r="I186" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J186" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
         <v>248</v>
       </c>
@@ -7840,8 +8411,11 @@
       <c r="I187" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J187" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
         <v>249</v>
       </c>
@@ -7870,8 +8444,11 @@
       <c r="I188" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J188" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
         <v>250</v>
       </c>
@@ -7900,8 +8477,11 @@
       <c r="I189" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J189" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
         <v>251</v>
       </c>
@@ -7930,8 +8510,11 @@
       <c r="I190" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J190" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
         <v>252</v>
       </c>
@@ -7960,8 +8543,11 @@
       <c r="I191" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J191" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
         <v>253</v>
       </c>
@@ -7990,8 +8576,11 @@
       <c r="I192" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J192" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
         <v>254</v>
       </c>
@@ -8020,8 +8609,11 @@
       <c r="I193" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J193" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
         <v>255</v>
       </c>
@@ -8050,8 +8642,11 @@
       <c r="I194" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J194" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
         <v>256</v>
       </c>
@@ -8080,8 +8675,11 @@
       <c r="I195" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J195" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
         <v>257</v>
       </c>
@@ -8110,8 +8708,11 @@
       <c r="I196" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J196" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
         <v>258</v>
       </c>
@@ -8140,8 +8741,11 @@
       <c r="I197" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J197" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
         <v>259</v>
       </c>
@@ -8170,8 +8774,11 @@
       <c r="I198" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J198" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
         <v>260</v>
       </c>
@@ -8200,8 +8807,11 @@
       <c r="I199" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J199" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
         <v>261</v>
       </c>
@@ -8230,8 +8840,11 @@
       <c r="I200" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J200" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
         <v>262</v>
       </c>
@@ -8260,8 +8873,11 @@
       <c r="I201" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J201" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
         <v>263</v>
       </c>
@@ -8290,8 +8906,11 @@
       <c r="I202" s="5" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J202" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
         <v>67</v>
       </c>
@@ -8320,8 +8939,11 @@
       <c r="I203" s="5" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J203" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
         <v>264</v>
       </c>
@@ -8350,8 +8972,11 @@
       <c r="I204" s="5" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J204" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
         <v>265</v>
       </c>
@@ -8380,8 +9005,11 @@
       <c r="I205" s="5" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J205" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
         <v>266</v>
       </c>
@@ -8410,8 +9038,11 @@
       <c r="I206" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J206" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
         <v>267</v>
       </c>
@@ -8440,8 +9071,11 @@
       <c r="I207" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J207" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
         <v>268</v>
       </c>
@@ -8470,8 +9104,11 @@
       <c r="I208" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J208" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
         <v>269</v>
       </c>
@@ -8500,8 +9137,11 @@
       <c r="I209" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J209" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
         <v>270</v>
       </c>
@@ -8530,8 +9170,11 @@
       <c r="I210" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J210" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
         <v>271</v>
       </c>
@@ -8560,8 +9203,11 @@
       <c r="I211" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J211" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
         <v>272</v>
       </c>
@@ -8590,8 +9236,11 @@
       <c r="I212" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J212" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
         <v>273</v>
       </c>
@@ -8620,8 +9269,11 @@
       <c r="I213" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J213" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
         <v>274</v>
       </c>
@@ -8650,8 +9302,11 @@
       <c r="I214" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J214" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
         <v>275</v>
       </c>
@@ -8680,8 +9335,11 @@
       <c r="I215" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J215" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
         <v>276</v>
       </c>
@@ -8710,8 +9368,11 @@
       <c r="I216" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J216" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
         <v>277</v>
       </c>
@@ -8740,8 +9401,11 @@
       <c r="I217" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J217" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
         <v>278</v>
       </c>
@@ -8770,8 +9434,11 @@
       <c r="I218" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J218" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
         <v>279</v>
       </c>
@@ -8800,8 +9467,11 @@
       <c r="I219" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J219" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
         <v>280</v>
       </c>
@@ -8830,8 +9500,11 @@
       <c r="I220" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J220" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
         <v>281</v>
       </c>
@@ -8860,8 +9533,11 @@
       <c r="I221" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J221" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
         <v>282</v>
       </c>
@@ -8890,8 +9566,11 @@
       <c r="I222" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J222" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
         <v>283</v>
       </c>
@@ -8920,8 +9599,11 @@
       <c r="I223" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J223" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
         <v>284</v>
       </c>
@@ -8950,8 +9632,11 @@
       <c r="I224" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J224" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
         <v>285</v>
       </c>
@@ -8980,8 +9665,11 @@
       <c r="I225" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J225" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
         <v>286</v>
       </c>
@@ -9010,8 +9698,11 @@
       <c r="I226" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J226" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
         <v>287</v>
       </c>
@@ -9040,8 +9731,11 @@
       <c r="I227" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J227" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
         <v>288</v>
       </c>
@@ -9070,8 +9764,11 @@
       <c r="I228" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J228" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
         <v>289</v>
       </c>
@@ -9100,8 +9797,11 @@
       <c r="I229" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J229" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
         <v>290</v>
       </c>
@@ -9130,8 +9830,11 @@
       <c r="I230" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J230" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
         <v>291</v>
       </c>
@@ -9160,8 +9863,11 @@
       <c r="I231" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J231" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
         <v>292</v>
       </c>
@@ -9190,8 +9896,11 @@
       <c r="I232" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J232" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
         <v>293</v>
       </c>
@@ -9220,8 +9929,11 @@
       <c r="I233" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J233" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
         <v>294</v>
       </c>
@@ -9250,8 +9962,11 @@
       <c r="I234" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J234" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
         <v>295</v>
       </c>
@@ -9280,8 +9995,11 @@
       <c r="I235" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J235" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="s">
         <v>296</v>
       </c>
@@ -9310,8 +10028,11 @@
       <c r="I236" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J236" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="s">
         <v>68</v>
       </c>
@@ -9340,8 +10061,11 @@
       <c r="I237" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J237" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="3" t="s">
         <v>69</v>
       </c>
@@ -9370,8 +10094,11 @@
       <c r="I238" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J238" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="3" t="s">
         <v>297</v>
       </c>
@@ -9400,8 +10127,11 @@
       <c r="I239" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J239" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="3" t="s">
         <v>298</v>
       </c>
@@ -9430,8 +10160,11 @@
       <c r="I240" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J240" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="s">
         <v>299</v>
       </c>
@@ -9460,8 +10193,11 @@
       <c r="I241" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J241" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
         <v>300</v>
       </c>
@@ -9490,8 +10226,11 @@
       <c r="I242" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J242" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="3" t="s">
         <v>301</v>
       </c>
@@ -9520,8 +10259,11 @@
       <c r="I243" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J243" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="3" t="s">
         <v>302</v>
       </c>
@@ -9550,8 +10292,11 @@
       <c r="I244" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J244" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="3" t="s">
         <v>303</v>
       </c>
@@ -9580,8 +10325,11 @@
       <c r="I245" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J245" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="3" t="s">
         <v>304</v>
       </c>
@@ -9610,8 +10358,11 @@
       <c r="I246" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J246" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="3" t="s">
         <v>305</v>
       </c>
@@ -9640,8 +10391,11 @@
       <c r="I247" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J247" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="3" t="s">
         <v>306</v>
       </c>
@@ -9670,8 +10424,11 @@
       <c r="I248" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J248" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" s="3" t="s">
         <v>307</v>
       </c>
@@ -9700,8 +10457,11 @@
       <c r="I249" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J249" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="3" t="s">
         <v>308</v>
       </c>
@@ -9730,8 +10490,11 @@
       <c r="I250" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J250" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" s="3" t="s">
         <v>309</v>
       </c>
@@ -9760,8 +10523,11 @@
       <c r="I251" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J251" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="3" t="s">
         <v>310</v>
       </c>
@@ -9790,8 +10556,11 @@
       <c r="I252" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J252" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="3" t="s">
         <v>311</v>
       </c>
@@ -9820,8 +10589,11 @@
       <c r="I253" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J253" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="3" t="s">
         <v>312</v>
       </c>
@@ -9850,8 +10622,11 @@
       <c r="I254" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J254" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" s="3" t="s">
         <v>313</v>
       </c>
@@ -9880,8 +10655,11 @@
       <c r="I255" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J255" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" s="3" t="s">
         <v>314</v>
       </c>
@@ -9910,8 +10688,11 @@
       <c r="I256" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J256" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="3" t="s">
         <v>315</v>
       </c>
@@ -9940,8 +10721,11 @@
       <c r="I257" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J257" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="3" t="s">
         <v>316</v>
       </c>
@@ -9970,8 +10754,11 @@
       <c r="I258" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J258" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="3" t="s">
         <v>317</v>
       </c>
@@ -10000,8 +10787,11 @@
       <c r="I259" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J259" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="3" t="s">
         <v>318</v>
       </c>
@@ -10030,8 +10820,11 @@
       <c r="I260" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J260" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="3" t="s">
         <v>319</v>
       </c>
@@ -10060,8 +10853,11 @@
       <c r="I261" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J261" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="3" t="s">
         <v>320</v>
       </c>
@@ -10090,8 +10886,11 @@
       <c r="I262" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J262" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="3" t="s">
         <v>321</v>
       </c>
@@ -10120,8 +10919,11 @@
       <c r="I263" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J263" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="3" t="s">
         <v>322</v>
       </c>
@@ -10150,8 +10952,11 @@
       <c r="I264" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J264" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="3" t="s">
         <v>323</v>
       </c>
@@ -10180,8 +10985,11 @@
       <c r="I265" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J265" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="3" t="s">
         <v>324</v>
       </c>
@@ -10210,8 +11018,11 @@
       <c r="I266" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J266" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="3" t="s">
         <v>325</v>
       </c>
@@ -10240,8 +11051,11 @@
       <c r="I267" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J267" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="3" t="s">
         <v>326</v>
       </c>
@@ -10270,8 +11084,11 @@
       <c r="I268" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J268" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="3" t="s">
         <v>327</v>
       </c>
@@ -10300,8 +11117,11 @@
       <c r="I269" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J269" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="3" t="s">
         <v>328</v>
       </c>
@@ -10330,8 +11150,11 @@
       <c r="I270" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J270" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="3" t="s">
         <v>329</v>
       </c>
@@ -10360,8 +11183,11 @@
       <c r="I271" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J271" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="3" t="s">
         <v>330</v>
       </c>
@@ -10390,8 +11216,11 @@
       <c r="I272" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J272" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" s="3" t="s">
         <v>331</v>
       </c>
@@ -10420,8 +11249,11 @@
       <c r="I273" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J273" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="3" t="s">
         <v>332</v>
       </c>
@@ -10450,8 +11282,11 @@
       <c r="I274" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J274" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="3" t="s">
         <v>333</v>
       </c>
@@ -10480,8 +11315,11 @@
       <c r="I275" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J275" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="3" t="s">
         <v>334</v>
       </c>
@@ -10510,8 +11348,11 @@
       <c r="I276" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J276" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="3" t="s">
         <v>335</v>
       </c>
@@ -10540,8 +11381,11 @@
       <c r="I277" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J277" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="3" t="s">
         <v>336</v>
       </c>
@@ -10570,8 +11414,11 @@
       <c r="I278" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J278" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" s="3" t="s">
         <v>337</v>
       </c>
@@ -10600,8 +11447,11 @@
       <c r="I279" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J279" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" s="3" t="s">
         <v>338</v>
       </c>
@@ -10630,8 +11480,11 @@
       <c r="I280" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J280" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" s="3" t="s">
         <v>339</v>
       </c>
@@ -10660,8 +11513,11 @@
       <c r="I281" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J281" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" s="3" t="s">
         <v>340</v>
       </c>
@@ -10690,8 +11546,11 @@
       <c r="I282" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J282" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" s="3" t="s">
         <v>341</v>
       </c>
@@ -10720,8 +11579,11 @@
       <c r="I283" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J283" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" s="3" t="s">
         <v>342</v>
       </c>
@@ -10750,8 +11612,11 @@
       <c r="I284" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J284" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" s="3" t="s">
         <v>343</v>
       </c>
@@ -10780,8 +11645,11 @@
       <c r="I285" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J285" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" s="3" t="s">
         <v>344</v>
       </c>
@@ -10810,8 +11678,11 @@
       <c r="I286" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J286" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" s="3" t="s">
         <v>345</v>
       </c>
@@ -10840,8 +11711,11 @@
       <c r="I287" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J287" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" s="3" t="s">
         <v>346</v>
       </c>
@@ -10870,8 +11744,11 @@
       <c r="I288" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J288" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" s="3" t="s">
         <v>347</v>
       </c>
@@ -10900,8 +11777,11 @@
       <c r="I289" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J289" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" s="3" t="s">
         <v>348</v>
       </c>
@@ -10930,8 +11810,11 @@
       <c r="I290" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J290" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" s="3" t="s">
         <v>349</v>
       </c>
@@ -10960,8 +11843,11 @@
       <c r="I291" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J291" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" s="3" t="s">
         <v>350</v>
       </c>
@@ -10990,8 +11876,11 @@
       <c r="I292" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J292" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" s="3" t="s">
         <v>351</v>
       </c>
@@ -11020,8 +11909,11 @@
       <c r="I293" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J293" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" s="3" t="s">
         <v>352</v>
       </c>
@@ -11050,8 +11942,11 @@
       <c r="I294" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J294" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" s="3" t="s">
         <v>353</v>
       </c>
@@ -11080,8 +11975,11 @@
       <c r="I295" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J295" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" s="3" t="s">
         <v>354</v>
       </c>
@@ -11110,8 +12008,11 @@
       <c r="I296" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J296" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" s="3" t="s">
         <v>355</v>
       </c>
@@ -11140,8 +12041,11 @@
       <c r="I297" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J297" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298" s="3" t="s">
         <v>356</v>
       </c>
@@ -11170,8 +12074,11 @@
       <c r="I298" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J298" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299" s="3" t="s">
         <v>357</v>
       </c>
@@ -11200,8 +12107,11 @@
       <c r="I299" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J299" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300" s="3" t="s">
         <v>358</v>
       </c>
@@ -11230,8 +12140,11 @@
       <c r="I300" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J300" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" s="3" t="s">
         <v>359</v>
       </c>
@@ -11260,8 +12173,11 @@
       <c r="I301" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J301" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302" s="3" t="s">
         <v>360</v>
       </c>
@@ -11290,8 +12206,11 @@
       <c r="I302" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J302" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A303" s="3" t="s">
         <v>361</v>
       </c>
@@ -11320,8 +12239,11 @@
       <c r="I303" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J303" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A304" s="3" t="s">
         <v>362</v>
       </c>
@@ -11350,8 +12272,11 @@
       <c r="I304" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J304" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A305" s="3" t="s">
         <v>363</v>
       </c>
@@ -11380,8 +12305,11 @@
       <c r="I305" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J305" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A306" s="3" t="s">
         <v>364</v>
       </c>
@@ -11410,8 +12338,11 @@
       <c r="I306" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J306" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A307" s="3" t="s">
         <v>365</v>
       </c>
@@ -11440,8 +12371,11 @@
       <c r="I307" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J307" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A308" s="3" t="s">
         <v>366</v>
       </c>
@@ -11470,8 +12404,11 @@
       <c r="I308" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J308" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A309" s="3" t="s">
         <v>367</v>
       </c>
@@ -11500,8 +12437,11 @@
       <c r="I309" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J309" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A310" s="3" t="s">
         <v>368</v>
       </c>
@@ -11530,8 +12470,11 @@
       <c r="I310" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J310" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A311" s="3" t="s">
         <v>369</v>
       </c>
@@ -11560,8 +12503,11 @@
       <c r="I311" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J311" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A312" s="3" t="s">
         <v>370</v>
       </c>
@@ -11590,8 +12536,11 @@
       <c r="I312" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J312" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A313" s="3" t="s">
         <v>371</v>
       </c>
@@ -11620,8 +12569,11 @@
       <c r="I313" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J313" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A314" s="3" t="s">
         <v>372</v>
       </c>
@@ -11650,8 +12602,11 @@
       <c r="I314" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J314" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A315" s="3" t="s">
         <v>373</v>
       </c>
@@ -11680,8 +12635,11 @@
       <c r="I315" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J315" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A316" s="3" t="s">
         <v>374</v>
       </c>
@@ -11710,8 +12668,11 @@
       <c r="I316" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J316" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A317" s="3" t="s">
         <v>375</v>
       </c>
@@ -11739,6 +12700,9 @@
       </c>
       <c r="I317" s="5" t="s">
         <v>20</v>
+      </c>
+      <c r="J317" t="s">
+        <v>421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fixes - Config
Fixed parameter limits when reading parameters from unit
Removed empty column A from excel sheet
Changed ReceiveTimeout back to 6000 after testing
</commit_message>
<xml_diff>
--- a/Booyco HMI Utility/Resources/Documents/CommanderParametersFile.xlsx
+++ b/Booyco HMI Utility/Resources/Documents/CommanderParametersFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Mernok Elektronik)\Mernok\Active\Git\SW\Booyco-HMI-Utility\Booyco HMI Utility\Resources\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB21D49-1605-4907-8C63-1F16D6B9269C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D523EF-A44F-45FF-9E53-4C9F91DB7191}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4442C273-631E-40E6-88D2-7449766A5078}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4442C273-631E-40E6-88D2-7449766A5078}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2355" uniqueCount="1099">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2368" uniqueCount="1099">
   <si>
     <t>Name</t>
   </si>
@@ -3792,8 +3792,8 @@
   <dimension ref="A1:P483"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F130" sqref="F130"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4831,7 +4831,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="3">
         <v>0</v>
@@ -9943,7 +9943,7 @@
         <v>1</v>
       </c>
       <c r="F160" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G160" s="3">
         <v>0</v>
@@ -20033,10 +20033,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AE2012-64ED-47D5-92F2-F7C5A6120600}">
-  <dimension ref="A1:K523"/>
+  <dimension ref="A1:L523"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20046,7 +20046,7 @@
     <col min="7" max="7" width="42.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>358</v>
       </c>
@@ -20060,7 +20060,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>501</v>
       </c>
@@ -20073,11 +20073,14 @@
       <c r="G2" t="s">
         <v>682</v>
       </c>
-      <c r="K2" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>507</v>
       </c>
@@ -20093,8 +20096,14 @@
       <c r="J3" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>511</v>
       </c>
@@ -20107,8 +20116,14 @@
       <c r="G4" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K4" s="1">
+        <v>2</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>513</v>
       </c>
@@ -20121,8 +20136,14 @@
       <c r="G5" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K5" s="1">
+        <v>3</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>525</v>
       </c>
@@ -20135,8 +20156,14 @@
       <c r="G6" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="1">
+        <v>4</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>495</v>
       </c>
@@ -20149,8 +20176,14 @@
       <c r="G7" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K7" s="1">
+        <v>5</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>538</v>
       </c>
@@ -20163,8 +20196,14 @@
       <c r="G8" t="s">
         <v>690</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K8" s="1">
+        <v>6</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>533</v>
       </c>
@@ -20174,8 +20213,14 @@
       <c r="G9" t="s">
         <v>691</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K9" s="1">
+        <v>7</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>508</v>
       </c>
@@ -20185,8 +20230,14 @@
       <c r="G10" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="1">
+        <v>8</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>509</v>
       </c>
@@ -20196,8 +20247,14 @@
       <c r="G11" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="1">
+        <v>9</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>510</v>
       </c>
@@ -20207,8 +20264,14 @@
       <c r="G12" t="s">
         <v>694</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="1">
+        <v>10</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>512</v>
       </c>
@@ -20218,8 +20281,14 @@
       <c r="G13" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="1">
+        <v>11</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>514</v>
       </c>
@@ -20229,8 +20298,14 @@
       <c r="G14" t="s">
         <v>696</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="1">
+        <v>12</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>515</v>
       </c>
@@ -20240,8 +20315,14 @@
       <c r="G15" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="1">
+        <v>13</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>516</v>
       </c>

</xml_diff>

<commit_message>
Config View Update - IP Conditioner, Data Grid
IP Conditioner added for IP fields in data grid
Data Grid Group and Sub Group is collapsed on view start-up
</commit_message>
<xml_diff>
--- a/Booyco HMI Utility/Resources/Documents/CommanderParametersFile.xlsx
+++ b/Booyco HMI Utility/Resources/Documents/CommanderParametersFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Mernok Elektronik)\Mernok\Active\Git\SW\Booyco-HMI-Utility\Booyco HMI Utility\Resources\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792E61DA-37A3-401A-AB8B-D70D01D585C5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654A88FD-3E4D-4B14-B664-DB8951F42DC8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4442C273-631E-40E6-88D2-7449766A5078}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4442C273-631E-40E6-88D2-7449766A5078}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3816,8 +3816,8 @@
   <dimension ref="A1:P483"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A341" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D352" sqref="D352"/>
+      <pane ySplit="1" topLeftCell="A464" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E481" sqref="E481"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18343,7 +18343,7 @@
       </c>
       <c r="B426" s="3">
         <f t="shared" si="10"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C426" s="3">
         <v>57</v>
@@ -18352,7 +18352,7 @@
         <v>46</v>
       </c>
       <c r="E426" s="3">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F426" s="3">
         <v>4</v>
@@ -18463,7 +18463,7 @@
       </c>
       <c r="B430" s="3">
         <f t="shared" si="10"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C430" s="3">
         <v>57</v>
@@ -18472,7 +18472,7 @@
         <v>46</v>
       </c>
       <c r="E430" s="3">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F430" s="3">
         <v>4</v>
@@ -18583,7 +18583,7 @@
       </c>
       <c r="B434" s="3">
         <f t="shared" si="10"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C434" s="3">
         <v>57</v>
@@ -18592,7 +18592,7 @@
         <v>46</v>
       </c>
       <c r="E434" s="3">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F434" s="3">
         <v>4</v>
@@ -18793,7 +18793,7 @@
       </c>
       <c r="B441" s="3">
         <f t="shared" si="10"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C441" s="3">
         <v>57</v>
@@ -18802,7 +18802,7 @@
         <v>46</v>
       </c>
       <c r="E441" s="3">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F441" s="3">
         <v>4</v>
@@ -18913,7 +18913,7 @@
       </c>
       <c r="B445" s="3">
         <f t="shared" si="10"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C445" s="3">
         <v>57</v>
@@ -18922,7 +18922,7 @@
         <v>46</v>
       </c>
       <c r="E445" s="3">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F445" s="3">
         <v>4</v>
@@ -19033,7 +19033,7 @@
       </c>
       <c r="B449" s="3">
         <f t="shared" si="10"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C449" s="3">
         <v>57</v>
@@ -19042,7 +19042,7 @@
         <v>46</v>
       </c>
       <c r="E449" s="3">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F449" s="3">
         <v>4</v>
@@ -19243,7 +19243,7 @@
       </c>
       <c r="B456" s="3">
         <f t="shared" si="10"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C456" s="3">
         <v>57</v>
@@ -19252,7 +19252,7 @@
         <v>46</v>
       </c>
       <c r="E456" s="3">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F456" s="3">
         <v>4</v>
@@ -19363,7 +19363,7 @@
       </c>
       <c r="B460" s="3">
         <f t="shared" si="10"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C460" s="3">
         <v>57</v>
@@ -19372,7 +19372,7 @@
         <v>46</v>
       </c>
       <c r="E460" s="3">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F460" s="3">
         <v>4</v>
@@ -19483,7 +19483,7 @@
       </c>
       <c r="B464" s="3">
         <f t="shared" si="10"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C464" s="3">
         <v>57</v>
@@ -19492,7 +19492,7 @@
         <v>46</v>
       </c>
       <c r="E464" s="3">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F464" s="3">
         <v>4</v>
@@ -19693,7 +19693,7 @@
       </c>
       <c r="B471" s="3">
         <f t="shared" si="10"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C471" s="3">
         <v>57</v>
@@ -19702,7 +19702,7 @@
         <v>46</v>
       </c>
       <c r="E471" s="3">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F471" s="3">
         <v>4</v>
@@ -19813,7 +19813,7 @@
       </c>
       <c r="B475" s="3">
         <f t="shared" si="10"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C475" s="3">
         <v>57</v>
@@ -19822,7 +19822,7 @@
         <v>46</v>
       </c>
       <c r="E475" s="3">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F475" s="3">
         <v>4</v>
@@ -19933,7 +19933,7 @@
       </c>
       <c r="B479" s="3">
         <f t="shared" si="10"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C479" s="3">
         <v>57</v>
@@ -19942,7 +19942,7 @@
         <v>46</v>
       </c>
       <c r="E479" s="3">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F479" s="3">
         <v>4</v>

</xml_diff>

<commit_message>
Parameter file update safety factor
</commit_message>
<xml_diff>
--- a/Booyco HMI Utility/Resources/Documents/CommanderParametersFile.xlsx
+++ b/Booyco HMI Utility/Resources/Documents/CommanderParametersFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mernok\DEVPRJ-168 (Booyco HMI)\Software\Booyco-HMI-Utility\Booyco HMI Utility\Resources\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43F23A8-A440-4D2A-9D84-650627459A63}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EC0EBD-71FB-483A-BD06-5D1209232E66}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4442C273-631E-40E6-88D2-7449766A5078}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4442C273-631E-40E6-88D2-7449766A5078}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3816,8 +3816,8 @@
   <dimension ref="A1:P483"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D280" sqref="D280"/>
+      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E200" sqref="E200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11310,17 +11310,16 @@
         <v>221</v>
       </c>
       <c r="B200" s="3">
-        <f t="shared" si="3"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C200" s="3">
-        <v>255</v>
+        <v>10000</v>
       </c>
       <c r="D200" s="3">
         <v>0</v>
       </c>
       <c r="E200" s="3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F200" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
Update Wifi heartbeat packet
Add Unix Timestamp in heartbeat
</commit_message>
<xml_diff>
--- a/Booyco HMI Utility/Resources/Documents/CommanderParametersFile.xlsx
+++ b/Booyco HMI Utility/Resources/Documents/CommanderParametersFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\Dropbox (Mernok Elektronik)\Mernok\DEVPRJ-168 (Booyco HMI)\Software\Github\Singlemachine\Booyco-HMI-Utility\Booyco HMI Utility\Resources\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B67504-950C-43D4-8D70-1B1BCBE5E05C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2C065A-11DA-4BB0-8337-BBA8587EEE45}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4442C273-631E-40E6-88D2-7449766A5078}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4442C273-631E-40E6-88D2-7449766A5078}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4031,8 +4031,8 @@
   <dimension ref="A1:P508"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A273" sqref="A273"/>
+      <pane ySplit="1" topLeftCell="A483" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I512" sqref="I512"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23279,10 +23279,10 @@
         <v>0</v>
       </c>
       <c r="H503" s="3" t="s">
-        <v>467</v>
+        <v>1122</v>
       </c>
       <c r="I503" s="3" t="s">
-        <v>472</v>
+        <v>1083</v>
       </c>
       <c r="J503" t="s">
         <v>317</v>
@@ -23468,10 +23468,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H4 H505:H508 H7:H35 H503 H41:H484" xr:uid="{EE42F429-08A4-4BE3-8F84-6536CE0CFC40}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H4 H505:H508 H7:H35 H41:H484" xr:uid="{EE42F429-08A4-4BE3-8F84-6536CE0CFC40}">
       <formula1>Groups</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H36:H40 I491:I493 H494:I502 H490:H493 H5:H6 I506:I508 I503 I2:I484" xr:uid="{7C24A3BA-34E6-47FE-B467-51CD70DB74D4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H36:H40 I491:I493 H494:I502 H490:H493 H5:H6 I506:I508 I2:I484" xr:uid="{7C24A3BA-34E6-47FE-B467-51CD70DB74D4}">
       <formula1>SubGroups</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>